<commit_message>
finished love house & hospital & activity filter
</commit_message>
<xml_diff>
--- a/iOS开发进度.xlsx
+++ b/iOS开发进度.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14240"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
   <si>
     <t>模块名称</t>
   </si>
@@ -104,10 +104,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>待调试</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>预计完成时间</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -116,14 +112,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>--</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11.05</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>11.08</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -132,47 +120,35 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>开发环境不允许，需等待数据联通</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>缺少图片</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>已调试大部分接口数据，缺少筛选页面设计</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>待调试，缺少账户设置设计图</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>UI尚需调整</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>11.10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>--</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11.11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11.12</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>待接通接口</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>11.14</t>
+    <t>11.13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11.16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11.13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11.15</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -276,8 +252,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -324,10 +306,12 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -674,7 +658,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -693,7 +677,7 @@
         <v>13</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>14</v>
@@ -710,7 +694,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>20</v>
@@ -724,7 +708,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>20</v>
@@ -738,7 +722,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>20</v>
@@ -752,7 +736,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>20</v>
@@ -766,7 +750,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>20</v>
@@ -780,7 +764,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>20</v>
@@ -790,14 +774,11 @@
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="1">
-        <v>0.9</v>
+      <c r="B8" s="9">
+        <v>1</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>20</v>
@@ -807,14 +788,11 @@
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="1">
-        <v>0.95</v>
+      <c r="B9" s="9">
+        <v>1</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>20</v>
@@ -824,14 +802,11 @@
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="1">
-        <v>0.95</v>
+      <c r="B10" s="9">
+        <v>1</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>20</v>
@@ -845,10 +820,10 @@
         <v>0.9</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>20</v>
@@ -862,7 +837,7 @@
         <v>0.3</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>20</v>
@@ -874,10 +849,7 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>20</v>
@@ -891,10 +863,10 @@
         <v>0.2</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>20</v>
@@ -906,10 +878,7 @@
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>20</v>
@@ -923,10 +892,7 @@
         <v>0.3</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>20</v>
@@ -940,10 +906,10 @@
         <v>0.9</v>
       </c>
       <c r="C17" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s">
         <v>25</v>
-      </c>
-      <c r="D17" t="s">
-        <v>29</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>20</v>
@@ -952,6 +918,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
finished user account setting view
</commit_message>
<xml_diff>
--- a/iOS开发进度.xlsx
+++ b/iOS开发进度.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
   <si>
     <t>模块名称</t>
   </si>
@@ -112,43 +112,39 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>11.08</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11.09</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>缺少图片</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>待调试，缺少账户设置设计图</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11.10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>待接通接口</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>11.16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>11.13</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>11.16</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11.13</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>11.15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分享</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11.18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11.17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11.14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>待切图</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -252,8 +248,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -306,12 +308,14 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -655,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -749,8 +753,8 @@
       <c r="B6" s="9">
         <v>1</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>24</v>
+      <c r="C6" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>20</v>
@@ -763,8 +767,8 @@
       <c r="B7" s="9">
         <v>1</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>23</v>
+      <c r="C7" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>20</v>
@@ -777,8 +781,8 @@
       <c r="B8" s="9">
         <v>1</v>
       </c>
-      <c r="C8" s="13" t="s">
-        <v>27</v>
+      <c r="C8" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>20</v>
@@ -791,8 +795,8 @@
       <c r="B9" s="9">
         <v>1</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>29</v>
+      <c r="C9" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>20</v>
@@ -805,8 +809,8 @@
       <c r="B10" s="9">
         <v>1</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>27</v>
+      <c r="C10" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>20</v>
@@ -816,15 +820,13 @@
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1">
-        <v>0.9</v>
+      <c r="B11" s="9">
+        <v>1</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>26</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D11" s="14"/>
       <c r="E11" s="7" t="s">
         <v>20</v>
       </c>
@@ -837,7 +839,7 @@
         <v>0.3</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>20</v>
@@ -849,7 +851,7 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="13" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>20</v>
@@ -860,13 +862,13 @@
         <v>19</v>
       </c>
       <c r="B14" s="1">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>20</v>
@@ -877,8 +879,8 @@
         <v>7</v>
       </c>
       <c r="B15" s="1"/>
-      <c r="C15" s="13" t="s">
-        <v>32</v>
+      <c r="C15" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>20</v>
@@ -892,7 +894,7 @@
         <v>0.3</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>20</v>
@@ -906,13 +908,24 @@
         <v>0.9</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished logins, weibo share
</commit_message>
<xml_diff>
--- a/iOS开发进度.xlsx
+++ b/iOS开发进度.xlsx
@@ -112,10 +112,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>待接通接口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>11.16</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -145,6 +141,10 @@
   </si>
   <si>
     <t>待切图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>待接通第三方登陆，KidsTC注册</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -248,8 +248,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -308,14 +314,16 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -662,7 +670,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -824,7 +832,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="7" t="s">
@@ -839,7 +847,7 @@
         <v>0.3</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>20</v>
@@ -849,9 +857,11 @@
       <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="1">
+        <v>0.1</v>
+      </c>
       <c r="C13" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>20</v>
@@ -861,14 +871,14 @@
       <c r="A14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="1">
-        <v>0.5</v>
+      <c r="B14" s="9">
+        <v>1</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>20</v>
@@ -894,7 +904,7 @@
         <v>0.3</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>20</v>
@@ -908,10 +918,10 @@
         <v>0.9</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>20</v>
@@ -919,13 +929,13 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="C18" s="13" t="s">
         <v>27</v>
-      </c>
-      <c r="B18" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add images, update role select, update news list
</commit_message>
<xml_diff>
--- a/iOS开发进度.xlsx
+++ b/iOS开发进度.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="30">
   <si>
     <t>模块名称</t>
   </si>
@@ -137,18 +137,6 @@
   </si>
   <si>
     <t>11.14</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>待切图</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>待接通第三方登陆，KidsTC注册</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>待确定分享数据源和内容调试</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -252,8 +240,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -318,16 +312,18 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -674,7 +670,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -861,8 +857,8 @@
       <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="1">
-        <v>0.3</v>
+      <c r="B13" s="9">
+        <v>1</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>25</v>
@@ -881,9 +877,6 @@
       <c r="C14" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D14" t="s">
-        <v>31</v>
-      </c>
       <c r="E14" s="7" t="s">
         <v>20</v>
       </c>
@@ -918,14 +911,11 @@
       <c r="A17" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="1">
-        <v>0.9</v>
+      <c r="B17" s="9">
+        <v>1</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>25</v>
-      </c>
-      <c r="D17" t="s">
-        <v>30</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>20</v>
@@ -935,14 +925,11 @@
       <c r="A18" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="1">
-        <v>0.9</v>
+      <c r="B18" s="9">
+        <v>1</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>27</v>
-      </c>
-      <c r="D18" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update service detail & store detail
</commit_message>
<xml_diff>
--- a/iOS开发进度.xlsx
+++ b/iOS开发进度.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
   <si>
     <t>模块名称</t>
   </si>
@@ -250,8 +250,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -362,7 +368,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="25">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
@@ -375,6 +381,7 @@
     <cellStyle name="访问过的超链接" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -386,6 +393,7 @@
     <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -732,7 +740,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -778,14 +786,11 @@
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="15">
-        <v>0.8</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>24</v>
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>20</v>

</xml_diff>